<commit_message>
hyrbid model with batch no2
</commit_message>
<xml_diff>
--- a/data/batch_no2/raw data/offline_data.xlsx
+++ b/data/batch_no2/raw data/offline_data.xlsx
@@ -1,35 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dxp2904\Downloads\Project_June_Ferm\hybrid-model-corynebacterium\data\batch_no2\raw data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5878D4C1-616C-4953-8C02-AD88FDEC3FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="BM" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet r:id="rId1" sheetId="1" name="BM"/>
+    <sheet r:id="rId2" sheetId="2" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -333,7 +314,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0000"/>
   </numFmts>
@@ -366,14 +347,14 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FFE7E6E6"/>
+      <color rgb="FFe7e6e6"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
-      <color rgb="FFE7E6E6"/>
+      <color rgb="FFe7e6e6"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -393,22 +374,22 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE7E6E6"/>
+        <fgColor rgb="FFe7e6e6"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEDEDED"/>
+        <fgColor rgb="FFededed"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFD966"/>
+        <fgColor rgb="FFffd966"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFBFBFBF"/>
+        <fgColor rgb="FFbfbfbf"/>
       </patternFill>
     </fill>
   </fills>
@@ -422,16 +403,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </left>
       <right style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </right>
       <top style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -446,144 +427,149 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="4" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="45">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="20" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="20" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="20" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="20" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="20" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="20" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="16" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="20" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="20" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="20" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="20" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="20" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="20" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="20" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -594,10 +580,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -635,71 +621,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -727,7 +713,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -750,11 +736,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -763,13 +749,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -779,7 +765,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -788,7 +774,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -797,7 +783,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -805,10 +791,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -873,78 +859,81 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="12.54296875" style="42" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="12.54296875" style="39" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17" style="42" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.26953125" style="44" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.54296875" style="39" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.7265625" style="39" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.54296875" style="39" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.7265625" style="39" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.1796875" style="39" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="13.54296875" style="39" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="38" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="39" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="39" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="39" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="39" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="39" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="39" width="17.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="44" width="19.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="39" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="39" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="39" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="39" width="17.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="39" width="12.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="39" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="39" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+      <c r="A1" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="47" t="s">
+      <c r="F1" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="G1" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="H1" s="48" t="s">
+      <c r="H1" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="I1" s="46" t="s">
+      <c r="I1" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="J1" s="46" t="s">
+      <c r="J1" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="K1" s="46" t="s">
+      <c r="K1" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="L1" s="46" t="s">
+      <c r="L1" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="M1" s="47" t="s">
+      <c r="M1" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="46" t="s">
+      <c r="N1" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="O1" s="46" t="s">
+      <c r="O1" s="8" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="23">
         <v>1</v>
       </c>
@@ -952,54 +941,46 @@
         <v>45</v>
       </c>
       <c r="C2" s="11">
-        <f t="shared" ref="C2:C14" si="0">B2/60</f>
-        <v>0.75</v>
+        <f>B2/60</f>
       </c>
       <c r="D2" s="11">
         <v>0.113</v>
       </c>
       <c r="E2" s="11">
         <f>D2*10</f>
-        <v>1.1300000000000001</v>
       </c>
       <c r="F2" s="11">
-        <f t="shared" ref="F2:F14" si="1">E2/3</f>
-        <v>0.37666666666666671</v>
+        <f>E2/3</f>
       </c>
       <c r="G2" s="11">
         <v>0</v>
       </c>
       <c r="H2" s="11">
-        <f t="shared" ref="H2:H14" si="2">(G2/1000)*350</f>
+        <f>(G2/1000)*350</f>
+      </c>
+      <c r="I2" s="11">
+        <v>4.177</v>
+      </c>
+      <c r="J2" s="11">
+        <f>(0.2354*I2)-0.544</f>
+      </c>
+      <c r="K2" s="11">
+        <f>I2*0.2267</f>
+      </c>
+      <c r="L2" s="11">
+        <f>K2*10</f>
+      </c>
+      <c r="M2" s="11">
+        <v>0.9481182119001622</v>
+      </c>
+      <c r="N2" s="11">
         <v>0</v>
       </c>
-      <c r="I2" s="11">
-        <v>4.1769999999999996</v>
-      </c>
-      <c r="J2" s="11">
-        <f t="shared" ref="J2:J14" si="3">(0.2354*I2)-0.544</f>
-        <v>0.43926579999999982</v>
-      </c>
-      <c r="K2" s="11">
-        <f t="shared" ref="K2:K14" si="4">I2*0.2267</f>
-        <v>0.94692589999999999</v>
-      </c>
-      <c r="L2" s="11">
-        <f t="shared" ref="L2:L14" si="5">K2*10</f>
-        <v>9.4692589999999992</v>
-      </c>
-      <c r="M2" s="24">
-        <v>0.94811821190016221</v>
-      </c>
-      <c r="N2" s="24">
-        <v>0</v>
-      </c>
-      <c r="O2" s="24">
-        <f t="shared" ref="O2:O13" si="6">(H3-H2)/(C3-C2)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O2" s="11">
+        <f>(H3-H2)/(C3-C2)</f>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="23">
         <v>2</v>
       </c>
@@ -1007,54 +988,46 @@
         <v>765</v>
       </c>
       <c r="C3" s="11">
-        <f t="shared" si="0"/>
-        <v>12.75</v>
+        <f>B3/60</f>
       </c>
       <c r="D3" s="11">
         <v>0.86</v>
       </c>
       <c r="E3" s="11">
         <f>D3*20</f>
-        <v>17.2</v>
       </c>
       <c r="F3" s="11">
-        <f t="shared" si="1"/>
-        <v>5.7333333333333334</v>
+        <f>E3/3</f>
       </c>
       <c r="G3" s="11">
         <v>0</v>
       </c>
       <c r="H3" s="11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>(G3/1000)*350</f>
       </c>
       <c r="I3" s="11">
         <v>1.599</v>
       </c>
       <c r="J3" s="11">
-        <f t="shared" si="3"/>
-        <v>-0.16759540000000006</v>
+        <f>(0.2354*I3)-0.544</f>
       </c>
       <c r="K3" s="11">
-        <f t="shared" si="4"/>
-        <v>0.36249330000000002</v>
+        <f>I3*0.2267</f>
       </c>
       <c r="L3" s="11">
-        <f t="shared" si="5"/>
-        <v>3.6249330000000004</v>
-      </c>
-      <c r="M3" s="24">
+        <f>K3*10</f>
+      </c>
+      <c r="M3" s="11">
         <v>0</v>
       </c>
-      <c r="N3" s="24">
+      <c r="N3" s="11">
         <v>0</v>
       </c>
-      <c r="O3" s="24">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O3" s="11">
+        <f>(H4-H3)/(C4-C3)</f>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="23">
         <v>3</v>
       </c>
@@ -1062,54 +1035,46 @@
         <v>855</v>
       </c>
       <c r="C4" s="11">
-        <f t="shared" si="0"/>
-        <v>14.25</v>
+        <f>B4/60</f>
       </c>
       <c r="D4" s="11">
         <v>0.86</v>
       </c>
       <c r="E4" s="11">
         <f>D4*20</f>
-        <v>17.2</v>
       </c>
       <c r="F4" s="11">
-        <f t="shared" si="1"/>
-        <v>5.7333333333333334</v>
+        <f>E4/3</f>
       </c>
       <c r="G4" s="11">
         <v>0</v>
       </c>
       <c r="H4" s="11">
-        <f t="shared" si="2"/>
+        <f>(G4/1000)*350</f>
+      </c>
+      <c r="I4" s="11">
+        <v>1.604</v>
+      </c>
+      <c r="J4" s="11">
+        <f>(0.2354*I4)-0.544</f>
+      </c>
+      <c r="K4" s="11">
+        <f>I4*0.2267</f>
+      </c>
+      <c r="L4" s="11">
+        <f>K4*10</f>
+      </c>
+      <c r="M4" s="11">
+        <v>0.4694110042230762</v>
+      </c>
+      <c r="N4" s="11">
         <v>0</v>
       </c>
-      <c r="I4" s="11">
-        <v>1.6040000000000001</v>
-      </c>
-      <c r="J4" s="11">
-        <f t="shared" si="3"/>
-        <v>-0.16641840000000002</v>
-      </c>
-      <c r="K4" s="11">
-        <f t="shared" si="4"/>
-        <v>0.36362680000000003</v>
-      </c>
-      <c r="L4" s="11">
-        <f t="shared" si="5"/>
-        <v>3.6362680000000003</v>
-      </c>
-      <c r="M4" s="24">
-        <v>0.46941100422307619</v>
-      </c>
-      <c r="N4" s="24">
-        <v>0</v>
-      </c>
-      <c r="O4" s="24">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O4" s="11">
+        <f>(H5-H4)/(C5-C4)</f>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="23">
         <v>4</v>
       </c>
@@ -1117,54 +1082,46 @@
         <v>946</v>
       </c>
       <c r="C5" s="11">
-        <f t="shared" si="0"/>
-        <v>15.766666666666667</v>
+        <f>B5/60</f>
       </c>
       <c r="D5" s="11">
         <v>0.9</v>
       </c>
       <c r="E5" s="11">
         <f>D5*20</f>
-        <v>18</v>
       </c>
       <c r="F5" s="11">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <f>E5/3</f>
       </c>
       <c r="G5" s="11">
         <v>0</v>
       </c>
       <c r="H5" s="11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>(G5/1000)*350</f>
       </c>
       <c r="I5" s="11">
         <v>1.639</v>
       </c>
       <c r="J5" s="11">
-        <f t="shared" si="3"/>
-        <v>-0.15817940000000003</v>
+        <f>(0.2354*I5)-0.544</f>
       </c>
       <c r="K5" s="11">
-        <f t="shared" si="4"/>
-        <v>0.37156130000000004</v>
+        <f>I5*0.2267</f>
       </c>
       <c r="L5" s="11">
-        <f t="shared" si="5"/>
-        <v>3.7156130000000003</v>
-      </c>
-      <c r="M5" s="24">
-        <v>0.69551268349480699</v>
-      </c>
-      <c r="N5" s="24">
+        <f>K5*10</f>
+      </c>
+      <c r="M5" s="11">
+        <v>0.695512683494807</v>
+      </c>
+      <c r="N5" s="11">
         <v>0</v>
       </c>
-      <c r="O5" s="24">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O5" s="11">
+        <f>(H6-H5)/(C6-C5)</f>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="23">
         <v>5</v>
       </c>
@@ -1172,54 +1129,46 @@
         <v>1005</v>
       </c>
       <c r="C6" s="11">
-        <f t="shared" si="0"/>
-        <v>16.75</v>
+        <f>B6/60</f>
       </c>
       <c r="D6" s="11">
-        <v>0.47849999999999998</v>
+        <v>0.4785</v>
       </c>
       <c r="E6" s="11">
-        <f t="shared" ref="E6:E13" si="7">D6*40</f>
-        <v>19.14</v>
+        <f>D6*40</f>
       </c>
       <c r="F6" s="11">
-        <f t="shared" si="1"/>
-        <v>6.38</v>
+        <f>E6/3</f>
       </c>
       <c r="G6" s="11">
         <v>0</v>
       </c>
       <c r="H6" s="11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>(G6/1000)*350</f>
       </c>
       <c r="I6" s="11">
         <v>1.577</v>
       </c>
       <c r="J6" s="11">
-        <f t="shared" si="3"/>
-        <v>-0.17277420000000004</v>
+        <f>(0.2354*I6)-0.544</f>
       </c>
       <c r="K6" s="11">
-        <f t="shared" si="4"/>
-        <v>0.35750589999999999</v>
+        <f>I6*0.2267</f>
       </c>
       <c r="L6" s="11">
-        <f t="shared" si="5"/>
-        <v>3.575059</v>
-      </c>
-      <c r="M6" s="24">
-        <v>0.52216249118444102</v>
-      </c>
-      <c r="N6" s="24">
+        <f>K6*10</f>
+      </c>
+      <c r="M6" s="11">
+        <v>0.522162491184441</v>
+      </c>
+      <c r="N6" s="11">
         <v>0</v>
       </c>
-      <c r="O6" s="24">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O6" s="11">
+        <f>(H7-H6)/(C7-C6)</f>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="23">
         <v>6</v>
       </c>
@@ -1227,54 +1176,46 @@
         <v>1095</v>
       </c>
       <c r="C7" s="11">
-        <f t="shared" si="0"/>
-        <v>18.25</v>
+        <f>B7/60</f>
       </c>
       <c r="D7" s="11">
-        <v>0.46500000000000002</v>
+        <v>0.465</v>
       </c>
       <c r="E7" s="11">
-        <f t="shared" si="7"/>
-        <v>18.600000000000001</v>
+        <f>D7*40</f>
       </c>
       <c r="F7" s="11">
-        <f t="shared" si="1"/>
-        <v>6.2</v>
+        <f>E7/3</f>
       </c>
       <c r="G7" s="11">
         <v>0</v>
       </c>
       <c r="H7" s="11">
-        <f t="shared" si="2"/>
+        <f>(G7/1000)*350</f>
+      </c>
+      <c r="I7" s="11">
+        <v>1.531</v>
+      </c>
+      <c r="J7" s="11">
+        <f>(0.2354*I7)-0.544</f>
+      </c>
+      <c r="K7" s="11">
+        <f>I7*0.2267</f>
+      </c>
+      <c r="L7" s="11">
+        <f>K7*10</f>
+      </c>
+      <c r="M7" s="11">
+        <v>0.5080659154413492</v>
+      </c>
+      <c r="N7" s="11">
         <v>0</v>
       </c>
-      <c r="I7" s="11">
-        <v>1.5309999999999999</v>
-      </c>
-      <c r="J7" s="11">
-        <f t="shared" si="3"/>
-        <v>-0.18360260000000006</v>
-      </c>
-      <c r="K7" s="11">
-        <f t="shared" si="4"/>
-        <v>0.34707769999999999</v>
-      </c>
-      <c r="L7" s="11">
-        <f t="shared" si="5"/>
-        <v>3.470777</v>
-      </c>
-      <c r="M7" s="24">
-        <v>0.50806591544134916</v>
-      </c>
-      <c r="N7" s="24">
-        <v>0</v>
-      </c>
-      <c r="O7" s="24">
-        <f t="shared" si="6"/>
-        <v>0.28000000000000003</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O7" s="11">
+        <f>(H8-H7)/(C8-C7)</f>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="23">
         <v>7</v>
       </c>
@@ -1282,55 +1223,46 @@
         <v>1170</v>
       </c>
       <c r="C8" s="11">
-        <f t="shared" si="0"/>
-        <v>19.5</v>
+        <f>B8/60</f>
       </c>
       <c r="D8" s="11">
         <v>0.45</v>
       </c>
       <c r="E8" s="11">
-        <f t="shared" si="7"/>
-        <v>18</v>
+        <f>D8*40</f>
       </c>
       <c r="F8" s="11">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <f>E8/3</f>
       </c>
       <c r="G8" s="11">
         <v>1</v>
       </c>
       <c r="H8" s="11">
-        <f t="shared" si="2"/>
-        <v>0.35000000000000003</v>
+        <f>(G8/1000)*350</f>
       </c>
       <c r="I8" s="11">
         <v>1.55</v>
       </c>
       <c r="J8" s="11">
-        <f t="shared" si="3"/>
-        <v>-0.17913000000000001</v>
+        <f>(0.2354*I8)-0.544</f>
       </c>
       <c r="K8" s="11">
-        <f t="shared" si="4"/>
-        <v>0.351385</v>
+        <f>I8*0.2267</f>
       </c>
       <c r="L8" s="11">
-        <f t="shared" si="5"/>
-        <v>3.5138500000000001</v>
-      </c>
-      <c r="M8" s="24">
+        <f>K8*10</f>
+      </c>
+      <c r="M8" s="11">
         <v>3.6648942359366705</v>
       </c>
-      <c r="N8" s="24">
-        <f t="shared" ref="N8:N13" si="8">(F9-F8)/H8</f>
-        <v>2.4761904761904772</v>
-      </c>
-      <c r="O8" s="24">
-        <f t="shared" si="6"/>
-        <v>3.02</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N8" s="11">
+        <f>(F9-F8)/H8</f>
+      </c>
+      <c r="O8" s="11">
+        <f>(H9-H8)/(C9-C8)</f>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="23">
         <v>8</v>
       </c>
@@ -1338,56 +1270,46 @@
         <v>1275</v>
       </c>
       <c r="C9" s="11">
-        <f t="shared" si="0"/>
-        <v>21.25</v>
+        <f>B9/60</f>
       </c>
       <c r="D9" s="11">
-        <v>0.51500000000000001</v>
+        <v>0.515</v>
       </c>
       <c r="E9" s="11">
-        <f t="shared" si="7"/>
-        <v>20.6</v>
+        <f>D9*40</f>
       </c>
       <c r="F9" s="11">
-        <f t="shared" si="1"/>
-        <v>6.8666666666666671</v>
+        <f>E9/3</f>
       </c>
       <c r="G9" s="11">
-        <f t="shared" ref="G9:G14" si="9">ABS(H20)</f>
-        <v>16.100000000000001</v>
+        <f>ABS(H20)</f>
       </c>
       <c r="H9" s="11">
-        <f t="shared" si="2"/>
-        <v>5.6349999999999998</v>
+        <f>(G9/1000)*350</f>
       </c>
       <c r="I9" s="11">
-        <v>1.3440000000000001</v>
+        <v>1.344</v>
       </c>
       <c r="J9" s="11">
-        <f t="shared" si="3"/>
-        <v>-0.2276224</v>
+        <f>(0.2354*I9)-0.544</f>
       </c>
       <c r="K9" s="11">
-        <f t="shared" si="4"/>
-        <v>0.30468480000000003</v>
+        <f>I9*0.2267</f>
       </c>
       <c r="L9" s="11">
-        <f t="shared" si="5"/>
-        <v>3.0468480000000002</v>
-      </c>
-      <c r="M9" s="24">
+        <f>K9*10</f>
+      </c>
+      <c r="M9" s="11">
         <v>1.0071116579248927</v>
       </c>
-      <c r="N9" s="24">
-        <f t="shared" si="8"/>
-        <v>5.9154096421177117E-2</v>
-      </c>
-      <c r="O9" s="24">
-        <f t="shared" si="6"/>
-        <v>1.4700000000000006</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N9" s="11">
+        <f>(F10-F9)/H9</f>
+      </c>
+      <c r="O9" s="11">
+        <f>(H10-H9)/(C10-C9)</f>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="23">
         <v>9</v>
       </c>
@@ -1395,56 +1317,46 @@
         <v>1335</v>
       </c>
       <c r="C10" s="11">
-        <f t="shared" si="0"/>
-        <v>22.25</v>
+        <f>B10/60</f>
       </c>
       <c r="D10" s="11">
         <v>0.54</v>
       </c>
       <c r="E10" s="11">
-        <f t="shared" si="7"/>
-        <v>21.6</v>
+        <f>D10*40</f>
       </c>
       <c r="F10" s="11">
-        <f t="shared" si="1"/>
-        <v>7.2</v>
+        <f>E10/3</f>
       </c>
       <c r="G10" s="11">
-        <f t="shared" si="9"/>
-        <v>20.3</v>
+        <f>ABS(H21)</f>
       </c>
       <c r="H10" s="11">
-        <f t="shared" si="2"/>
-        <v>7.1050000000000004</v>
+        <f>(G10/1000)*350</f>
       </c>
       <c r="I10" s="11">
-        <v>1.6839999999999999</v>
+        <v>1.684</v>
       </c>
       <c r="J10" s="11">
-        <f t="shared" si="3"/>
-        <v>-0.14758640000000006</v>
+        <f>(0.2354*I10)-0.544</f>
       </c>
       <c r="K10" s="11">
-        <f t="shared" si="4"/>
-        <v>0.38176280000000001</v>
+        <f>I10*0.2267</f>
       </c>
       <c r="L10" s="11">
-        <f t="shared" si="5"/>
-        <v>3.817628</v>
-      </c>
-      <c r="M10" s="24">
+        <f>K10*10</f>
+      </c>
+      <c r="M10" s="11">
         <v>5.7731520165793855</v>
       </c>
-      <c r="N10" s="24">
-        <f t="shared" si="8"/>
-        <v>0.30025803424818209</v>
-      </c>
-      <c r="O10" s="24">
-        <f t="shared" si="6"/>
-        <v>7.9449999999999985</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N10" s="11">
+        <f>(F11-F10)/H10</f>
+      </c>
+      <c r="O10" s="11">
+        <f>(H11-H10)/(C11-C10)</f>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="23">
         <v>10</v>
       </c>
@@ -1452,56 +1364,46 @@
         <v>1395</v>
       </c>
       <c r="C11" s="11">
-        <f t="shared" si="0"/>
-        <v>23.25</v>
+        <f>B11/60</f>
       </c>
       <c r="D11" s="11">
         <v>0.7</v>
       </c>
       <c r="E11" s="11">
-        <f t="shared" si="7"/>
-        <v>28</v>
+        <f>D11*40</f>
       </c>
       <c r="F11" s="11">
-        <f t="shared" si="1"/>
-        <v>9.3333333333333339</v>
+        <f>E11/3</f>
       </c>
       <c r="G11" s="11">
-        <f t="shared" si="9"/>
-        <v>43</v>
+        <f>ABS(H22)</f>
       </c>
       <c r="H11" s="11">
-        <f t="shared" si="2"/>
-        <v>15.049999999999999</v>
+        <f>(G11/1000)*350</f>
       </c>
       <c r="I11" s="11">
-        <v>1.4770000000000001</v>
+        <v>1.477</v>
       </c>
       <c r="J11" s="11">
-        <f t="shared" si="3"/>
-        <v>-0.19631419999999999</v>
+        <f>(0.2354*I11)-0.544</f>
       </c>
       <c r="K11" s="11">
-        <f t="shared" si="4"/>
-        <v>0.33483590000000002</v>
+        <f>I11*0.2267</f>
       </c>
       <c r="L11" s="11">
-        <f t="shared" si="5"/>
-        <v>3.3483590000000003</v>
-      </c>
-      <c r="M11" s="24">
-        <v>0.64770834284972345</v>
-      </c>
-      <c r="N11" s="24">
-        <f t="shared" si="8"/>
-        <v>9.7452934662237117E-2</v>
-      </c>
-      <c r="O11" s="24">
-        <f t="shared" si="6"/>
-        <v>6.0550000000000015</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <f>K11*10</f>
+      </c>
+      <c r="M11" s="11">
+        <v>0.6477083428497235</v>
+      </c>
+      <c r="N11" s="11">
+        <f>(F12-F11)/H11</f>
+      </c>
+      <c r="O11" s="11">
+        <f>(H12-H11)/(C12-C11)</f>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="23">
         <v>11</v>
       </c>
@@ -1509,56 +1411,46 @@
         <v>1455</v>
       </c>
       <c r="C12" s="11">
-        <f t="shared" si="0"/>
-        <v>24.25</v>
+        <f>B12/60</f>
       </c>
       <c r="D12" s="11">
         <v>0.81</v>
       </c>
       <c r="E12" s="11">
-        <f t="shared" si="7"/>
-        <v>32.400000000000006</v>
+        <f>D12*40</f>
       </c>
       <c r="F12" s="11">
-        <f t="shared" si="1"/>
-        <v>10.800000000000002</v>
+        <f>E12/3</f>
       </c>
       <c r="G12" s="11">
-        <f t="shared" si="9"/>
-        <v>60.3</v>
+        <f>ABS(H23)</f>
       </c>
       <c r="H12" s="11">
-        <f t="shared" si="2"/>
-        <v>21.105</v>
+        <f>(G12/1000)*350</f>
       </c>
       <c r="I12" s="11">
-        <v>1.6679999999999999</v>
+        <v>1.668</v>
       </c>
       <c r="J12" s="11">
-        <f t="shared" si="3"/>
-        <v>-0.15135280000000007</v>
+        <f>(0.2354*I12)-0.544</f>
       </c>
       <c r="K12" s="11">
-        <f t="shared" si="4"/>
-        <v>0.37813560000000002</v>
+        <f>I12*0.2267</f>
       </c>
       <c r="L12" s="11">
-        <f t="shared" si="5"/>
-        <v>3.7813560000000002</v>
-      </c>
-      <c r="M12" s="24">
-        <v>3.9435362401171079</v>
-      </c>
-      <c r="N12" s="24">
-        <f t="shared" si="8"/>
-        <v>7.4547895443417778E-2</v>
-      </c>
-      <c r="O12" s="24">
-        <f t="shared" si="6"/>
-        <v>9.66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <f>K12*10</f>
+      </c>
+      <c r="M12" s="11">
+        <v>3.943536240117108</v>
+      </c>
+      <c r="N12" s="11">
+        <f>(F13-F12)/H12</f>
+      </c>
+      <c r="O12" s="11">
+        <f>(H13-H12)/(C13-C12)</f>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="23">
         <v>12</v>
       </c>
@@ -1566,56 +1458,46 @@
         <v>1515</v>
       </c>
       <c r="C13" s="11">
-        <f t="shared" si="0"/>
-        <v>25.25</v>
+        <f>B13/60</f>
       </c>
       <c r="D13" s="11">
-        <v>0.92800000000000005</v>
+        <v>0.928</v>
       </c>
       <c r="E13" s="11">
-        <f t="shared" si="7"/>
-        <v>37.120000000000005</v>
+        <f>D13*40</f>
       </c>
       <c r="F13" s="11">
-        <f t="shared" si="1"/>
-        <v>12.373333333333335</v>
+        <f>E13/3</f>
       </c>
       <c r="G13" s="11">
-        <f t="shared" si="9"/>
-        <v>87.9</v>
+        <f>ABS(H24)</f>
       </c>
       <c r="H13" s="11">
-        <f t="shared" si="2"/>
-        <v>30.765000000000001</v>
+        <f>(G13/1000)*350</f>
       </c>
       <c r="I13" s="11">
         <v>1.829</v>
       </c>
       <c r="J13" s="11">
-        <f t="shared" si="3"/>
-        <v>-0.11345340000000004</v>
+        <f>(0.2354*I13)-0.544</f>
       </c>
       <c r="K13" s="11">
-        <f t="shared" si="4"/>
-        <v>0.41463430000000001</v>
+        <f>I13*0.2267</f>
       </c>
       <c r="L13" s="11">
-        <f t="shared" si="5"/>
-        <v>4.1463429999999999</v>
-      </c>
-      <c r="M13" s="24">
-        <v>2.5372188316163391</v>
-      </c>
-      <c r="N13" s="24">
-        <f t="shared" si="8"/>
-        <v>0.56861151741697824</v>
-      </c>
-      <c r="O13" s="24">
-        <f t="shared" si="6"/>
-        <v>10.117142857142856</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <f>K13*10</f>
+      </c>
+      <c r="M13" s="11">
+        <v>2.537218831616339</v>
+      </c>
+      <c r="N13" s="11">
+        <f>(F14-F13)/H13</f>
+      </c>
+      <c r="O13" s="11">
+        <f>(H14-H13)/(C14-C13)</f>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="23">
         <v>13</v>
       </c>
@@ -1623,45 +1505,40 @@
         <v>2250</v>
       </c>
       <c r="C14" s="11">
-        <f t="shared" si="0"/>
-        <v>37.5</v>
+        <f>B14/60</f>
       </c>
       <c r="D14" s="11">
-        <v>0.56000000000000005</v>
+        <v>0.56</v>
       </c>
       <c r="E14" s="11">
         <f>D14*160</f>
-        <v>89.600000000000009</v>
       </c>
       <c r="F14" s="11">
-        <f t="shared" si="1"/>
-        <v>29.866666666666671</v>
+        <f>E14/3</f>
       </c>
       <c r="G14" s="11">
-        <f t="shared" si="9"/>
-        <v>442</v>
+        <f>ABS(H25)</f>
       </c>
       <c r="H14" s="11">
-        <f t="shared" si="2"/>
-        <v>154.69999999999999</v>
+        <f>(G14/1000)*350</f>
       </c>
       <c r="I14" s="11">
         <v>1.63</v>
       </c>
       <c r="J14" s="11">
-        <f t="shared" si="3"/>
-        <v>-0.16029800000000005</v>
+        <f>(0.2354*I14)-0.544</f>
       </c>
       <c r="K14" s="11">
-        <f t="shared" si="4"/>
-        <v>0.36952099999999999</v>
+        <f>I14*0.2267</f>
       </c>
       <c r="L14" s="11">
-        <f t="shared" si="5"/>
-        <v>3.6952099999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <f>K14*10</f>
+      </c>
+      <c r="M14" s="43"/>
+      <c r="N14" s="43"/>
+      <c r="O14" s="43"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="7"/>
@@ -1669,7 +1546,7 @@
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="6"/>
-      <c r="H15" s="43"/>
+      <c r="H15" s="6"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
@@ -1678,7 +1555,7 @@
       <c r="N15" s="7"/>
       <c r="O15" s="7"/>
     </row>
-    <row r="16" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="7"/>
@@ -1686,7 +1563,7 @@
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="6"/>
-      <c r="H16" s="43"/>
+      <c r="H16" s="6"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
@@ -1695,7 +1572,7 @@
       <c r="N16" s="7"/>
       <c r="O16" s="7"/>
     </row>
-    <row r="17" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
@@ -1703,7 +1580,7 @@
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="6"/>
-      <c r="H17" s="43"/>
+      <c r="H17" s="6"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
@@ -1712,7 +1589,7 @@
       <c r="N17" s="7"/>
       <c r="O17" s="7"/>
     </row>
-    <row r="18" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="7"/>
@@ -1720,7 +1597,7 @@
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="6"/>
-      <c r="H18" s="43"/>
+      <c r="H18" s="6"/>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
@@ -1729,7 +1606,7 @@
       <c r="N18" s="7"/>
       <c r="O18" s="7"/>
     </row>
-    <row r="19" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="7"/>
@@ -1737,7 +1614,7 @@
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43"/>
+      <c r="H19" s="6"/>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
@@ -1746,7 +1623,7 @@
       <c r="N19" s="7"/>
       <c r="O19" s="7"/>
     </row>
-    <row r="20" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
@@ -1755,7 +1632,7 @@
       <c r="F20" s="7"/>
       <c r="G20" s="6"/>
       <c r="H20" s="11">
-        <v>-16.100000000000001</v>
+        <v>-16.1</v>
       </c>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
@@ -1765,7 +1642,7 @@
       <c r="N20" s="7"/>
       <c r="O20" s="7"/>
     </row>
-    <row r="21" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="7"/>
@@ -1784,7 +1661,7 @@
       <c r="N21" s="7"/>
       <c r="O21" s="7"/>
     </row>
-    <row r="22" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="7"/>
@@ -1803,7 +1680,7 @@
       <c r="N22" s="7"/>
       <c r="O22" s="7"/>
     </row>
-    <row r="23" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="7"/>
@@ -1822,7 +1699,7 @@
       <c r="N23" s="7"/>
       <c r="O23" s="7"/>
     </row>
-    <row r="24" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="7"/>
@@ -1841,7 +1718,7 @@
       <c r="N24" s="7"/>
       <c r="O24" s="7"/>
     </row>
-    <row r="25" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="7"/>
@@ -1862,15 +1739,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Calibri"&amp;10&amp;K000000 Public&amp;1#_x000D_</oddHeader>
-    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public</oddFooter>
-  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1878,26 +1751,33 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.54296875" style="38" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.26953125" style="39" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.26953125" style="39" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7265625" style="39" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12.54296875" style="38" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7265625" style="38" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.81640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.26953125" style="41" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.81640625" style="42" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.26953125" style="42" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.81640625" style="39" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.54296875" style="41" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.81640625" style="39" bestFit="1" customWidth="1"/>
-    <col min="15" max="20" width="12.54296875" style="39" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="12.54296875" style="38" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="34" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="35" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="35" width="12.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="35" width="19.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="34" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="34" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="34" width="14.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="36" width="16.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="37" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="38" width="16.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="38" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="39" width="18.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="37" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="39" width="13.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="39" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="39" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="39" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="39" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="39" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="39" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="34" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="34" width="12.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1929,7 +1809,7 @@
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
     </row>
-    <row r="2" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="1"/>
       <c r="B2" s="8" t="s">
         <v>4</v>
@@ -1959,15 +1839,15 @@
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
     </row>
-    <row r="3" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
       <c r="A3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="11">
-        <v>1.0468999999999999</v>
+        <v>1.0469</v>
       </c>
       <c r="C3" s="11">
-        <v>1.0497000000000001</v>
+        <v>1.0497</v>
       </c>
       <c r="D3" s="11">
         <v>1.0603</v>
@@ -1991,7 +1871,7 @@
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
     </row>
-    <row r="4" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
       <c r="A4" s="12" t="s">
         <v>8</v>
       </c>
@@ -2017,7 +1897,7 @@
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
     </row>
-    <row r="5" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
       <c r="A5" s="1"/>
       <c r="B5" s="8" t="s">
         <v>9</v>
@@ -2073,7 +1953,7 @@
       <c r="U5" s="13"/>
       <c r="V5" s="19"/>
     </row>
-    <row r="6" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
       <c r="A6" s="10" t="s">
         <v>7</v>
       </c>
@@ -2081,10 +1961,10 @@
         <v>1.06</v>
       </c>
       <c r="C6" s="11">
-        <v>1.0609999999999999</v>
+        <v>1.061</v>
       </c>
       <c r="D6" s="11">
-        <v>1.0630999999999999</v>
+        <v>1.0631</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -2095,50 +1975,43 @@
         <v>26</v>
       </c>
       <c r="I6" s="22">
-        <v>2.8125</v>
+        <v>3.8125</v>
       </c>
       <c r="J6" s="23">
         <v>45</v>
       </c>
       <c r="K6" s="23">
-        <f t="shared" ref="K6:K18" si="0">J6*60</f>
-        <v>2700</v>
+        <f>J6*60</f>
       </c>
       <c r="L6" s="11">
-        <f t="shared" ref="L6:L18" si="1">J6/60</f>
-        <v>0.75</v>
+        <f>J6/60</f>
       </c>
       <c r="M6" s="22">
-        <v>2.0486111111111112</v>
+        <v>3.048611111111111</v>
       </c>
       <c r="N6" s="11">
         <v>0.113</v>
       </c>
       <c r="O6" s="11">
         <f>N6*10</f>
-        <v>1.1300000000000001</v>
       </c>
       <c r="P6" s="11">
-        <f t="shared" ref="P6:P18" si="2">O6/3</f>
-        <v>0.37666666666666671</v>
-      </c>
-      <c r="Q6" s="24">
-        <f t="shared" ref="Q6:Q17" si="3">ABS(P7-P6)/ABS(L7-L6)</f>
-        <v>0.42853333333333332</v>
-      </c>
-      <c r="R6" s="24">
-        <f t="shared" ref="R6:R17" si="4">ABS(LN(P7/P6))/ABS(LN(L7/L6))</f>
-        <v>0.94811821190016221</v>
-      </c>
-      <c r="S6" s="24">
-        <f t="shared" ref="S6:S17" si="5">(LN(P7/P6))/(LN(L7/L6))</f>
-        <v>0.94811821190016221</v>
+        <f>O6/3</f>
+      </c>
+      <c r="Q6" s="11">
+        <f>ABS(P7-P6)/ABS(L7-L6)</f>
+      </c>
+      <c r="R6" s="11">
+        <f>ABS(LN(P7/P6))/ABS(LN(L7/L6))</f>
+      </c>
+      <c r="S6" s="11">
+        <f>(LN(P7/P6))/(LN(L7/L6))</f>
       </c>
       <c r="T6" s="7"/>
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
     </row>
-    <row r="7" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
       <c r="A7" s="12" t="s">
         <v>8</v>
       </c>
@@ -2150,54 +2023,47 @@
       <c r="G7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="25" t="s">
+      <c r="H7" s="21" t="s">
         <v>28</v>
       </c>
       <c r="I7" s="22">
-        <v>2.333333333333333</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="J7" s="23">
         <v>795</v>
       </c>
       <c r="K7" s="23">
-        <f t="shared" si="0"/>
-        <v>47700</v>
+        <f>J7*60</f>
       </c>
       <c r="L7" s="11">
-        <f t="shared" si="1"/>
-        <v>13.25</v>
+        <f>J7/60</f>
       </c>
       <c r="M7" s="22">
-        <v>2.0555555555555554</v>
+        <v>3.0555555555555554</v>
       </c>
       <c r="N7" s="11">
         <v>0.86</v>
       </c>
       <c r="O7" s="11">
         <f>N7*20</f>
-        <v>17.2</v>
       </c>
       <c r="P7" s="11">
-        <f t="shared" si="2"/>
-        <v>5.7333333333333334</v>
-      </c>
-      <c r="Q7" s="26">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="R7" s="26">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="S7" s="26">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f>O7/3</f>
+      </c>
+      <c r="Q7" s="23">
+        <f>ABS(P8-P7)/ABS(L8-L7)</f>
+      </c>
+      <c r="R7" s="23">
+        <f>ABS(LN(P8/P7))/ABS(LN(L8/L7))</f>
+      </c>
+      <c r="S7" s="23">
+        <f>(LN(P8/P7))/(LN(L8/L7))</f>
       </c>
       <c r="T7" s="7"/>
       <c r="U7" s="1"/>
       <c r="V7" s="1"/>
     </row>
-    <row r="8" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
       <c r="A8" s="1"/>
       <c r="B8" s="8" t="s">
         <v>29</v>
@@ -2213,54 +2079,47 @@
       <c r="G8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H8" s="25" t="s">
+      <c r="H8" s="21" t="s">
         <v>28</v>
       </c>
       <c r="I8" s="22">
-        <v>2.395833333333333</v>
+        <v>3.3958333333333335</v>
       </c>
       <c r="J8" s="23">
         <v>885</v>
       </c>
       <c r="K8" s="23">
-        <f t="shared" si="0"/>
-        <v>53100</v>
+        <f>J8*60</f>
       </c>
       <c r="L8" s="11">
-        <f t="shared" si="1"/>
-        <v>14.75</v>
+        <f>J8/60</f>
       </c>
       <c r="M8" s="22">
-        <v>2.0555555555555554</v>
+        <v>3.0555555555555554</v>
       </c>
       <c r="N8" s="11">
         <v>0.86</v>
       </c>
       <c r="O8" s="11">
         <f>N8*20</f>
-        <v>17.2</v>
       </c>
       <c r="P8" s="11">
-        <f t="shared" si="2"/>
-        <v>5.7333333333333334</v>
-      </c>
-      <c r="Q8" s="24">
-        <f t="shared" si="3"/>
-        <v>0.17777777777777773</v>
-      </c>
-      <c r="R8" s="24">
-        <f t="shared" si="4"/>
-        <v>0.46941100422307619</v>
-      </c>
-      <c r="S8" s="24">
-        <f t="shared" si="5"/>
-        <v>0.46941100422307619</v>
+        <f>O8/3</f>
+      </c>
+      <c r="Q8" s="11">
+        <f>ABS(P9-P8)/ABS(L9-L8)</f>
+      </c>
+      <c r="R8" s="11">
+        <f>ABS(LN(P9/P8))/ABS(LN(L9/L8))</f>
+      </c>
+      <c r="S8" s="11">
+        <f>(LN(P9/P8))/(LN(L9/L8))</f>
       </c>
       <c r="T8" s="7"/>
       <c r="U8" s="1"/>
       <c r="V8" s="1"/>
     </row>
-    <row r="9" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
       <c r="A9" s="10" t="s">
         <v>7</v>
       </c>
@@ -2268,7 +2127,7 @@
         <v>1.0566</v>
       </c>
       <c r="C9" s="11">
-        <v>1.0470999999999999</v>
+        <v>1.0471</v>
       </c>
       <c r="D9" s="11">
         <v>1.0628</v>
@@ -2278,54 +2137,47 @@
       <c r="G9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="H9" s="21" t="s">
         <v>33</v>
       </c>
       <c r="I9" s="22">
-        <v>2.458333333333333</v>
+        <v>3.4583333333333335</v>
       </c>
       <c r="J9" s="23">
         <v>975</v>
       </c>
       <c r="K9" s="23">
-        <f t="shared" si="0"/>
-        <v>58500</v>
+        <f>J9*60</f>
       </c>
       <c r="L9" s="11">
-        <f t="shared" si="1"/>
-        <v>16.25</v>
+        <f>J9/60</f>
       </c>
       <c r="M9" s="22">
-        <v>2.0555555555555554</v>
+        <v>3.0555555555555554</v>
       </c>
       <c r="N9" s="11">
         <v>0.9</v>
       </c>
       <c r="O9" s="23">
         <f>N9*20</f>
-        <v>18</v>
       </c>
       <c r="P9" s="23">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="Q9" s="24">
-        <f t="shared" si="3"/>
-        <v>0.25333333333333324</v>
-      </c>
-      <c r="R9" s="24">
-        <f t="shared" si="4"/>
-        <v>0.69551268349480699</v>
-      </c>
-      <c r="S9" s="24">
-        <f t="shared" si="5"/>
-        <v>0.69551268349480699</v>
+        <f>O9/3</f>
+      </c>
+      <c r="Q9" s="11">
+        <f>ABS(P10-P9)/ABS(L10-L9)</f>
+      </c>
+      <c r="R9" s="11">
+        <f>ABS(LN(P10/P9))/ABS(LN(L10/L9))</f>
+      </c>
+      <c r="S9" s="11">
+        <f>(LN(P10/P9))/(LN(L10/L9))</f>
       </c>
       <c r="T9" s="7"/>
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
     </row>
-    <row r="10" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
       <c r="A10" s="12" t="s">
         <v>8</v>
       </c>
@@ -2337,111 +2189,97 @@
       <c r="G10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H10" s="25" t="s">
+      <c r="H10" s="21" t="s">
         <v>28</v>
       </c>
       <c r="I10" s="22">
-        <v>2.520833333333333</v>
+        <v>3.5208333333333335</v>
       </c>
       <c r="J10" s="23">
         <v>1065</v>
       </c>
       <c r="K10" s="23">
-        <f t="shared" si="0"/>
-        <v>63900</v>
+        <f>J10*60</f>
       </c>
       <c r="L10" s="11">
-        <f t="shared" si="1"/>
-        <v>17.75</v>
-      </c>
-      <c r="M10" s="27">
-        <v>2.0694444444444446</v>
+        <f>J10/60</f>
+      </c>
+      <c r="M10" s="24">
+        <v>3.0694444444444446</v>
       </c>
       <c r="N10" s="11">
-        <v>0.47849999999999998</v>
+        <v>0.4785</v>
       </c>
       <c r="O10" s="11">
-        <f t="shared" ref="O10:O17" si="6">N10*40</f>
-        <v>19.14</v>
+        <f>N10*40</f>
       </c>
       <c r="P10" s="11">
-        <f t="shared" si="2"/>
-        <v>6.38</v>
-      </c>
-      <c r="Q10" s="24">
-        <f t="shared" si="3"/>
-        <v>0.17999999999999972</v>
-      </c>
-      <c r="R10" s="24">
-        <f t="shared" si="4"/>
-        <v>0.52216249118444102</v>
-      </c>
-      <c r="S10" s="24">
-        <f t="shared" si="5"/>
-        <v>-0.52216249118444102</v>
+        <f>O10/3</f>
+      </c>
+      <c r="Q10" s="11">
+        <f>ABS(P11-P10)/ABS(L11-L10)</f>
+      </c>
+      <c r="R10" s="11">
+        <f>ABS(LN(P11/P10))/ABS(LN(L11/L10))</f>
+      </c>
+      <c r="S10" s="11">
+        <f>(LN(P11/P10))/(LN(L11/L10))</f>
       </c>
       <c r="T10" s="7"/>
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
     </row>
-    <row r="11" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
       <c r="A11" s="1"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="28" t="s">
+      <c r="G11" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="25" t="s">
+      <c r="H11" s="21" t="s">
         <v>33</v>
       </c>
       <c r="I11" s="22">
-        <v>2.5625</v>
+        <v>3.5625</v>
       </c>
       <c r="J11" s="23">
         <v>1125</v>
       </c>
       <c r="K11" s="23">
-        <f t="shared" si="0"/>
-        <v>67500</v>
+        <f>J11*60</f>
       </c>
       <c r="L11" s="11">
-        <f t="shared" si="1"/>
-        <v>18.75</v>
+        <f>J11/60</f>
       </c>
       <c r="M11" s="22">
-        <v>2.0694444444444446</v>
+        <v>3.0694444444444446</v>
       </c>
       <c r="N11" s="11">
-        <v>0.46500000000000002</v>
+        <v>0.465</v>
       </c>
       <c r="O11" s="11">
-        <f t="shared" si="6"/>
-        <v>18.600000000000001</v>
+        <f>N11*40</f>
       </c>
       <c r="P11" s="11">
-        <f t="shared" si="2"/>
-        <v>6.2</v>
-      </c>
-      <c r="Q11" s="24">
-        <f t="shared" si="3"/>
-        <v>0.16000000000000014</v>
-      </c>
-      <c r="R11" s="24">
-        <f t="shared" si="4"/>
-        <v>0.50806591544134916</v>
-      </c>
-      <c r="S11" s="24">
-        <f t="shared" si="5"/>
-        <v>-0.50806591544134916</v>
+        <f>O11/3</f>
+      </c>
+      <c r="Q11" s="11">
+        <f>ABS(P12-P11)/ABS(L12-L11)</f>
+      </c>
+      <c r="R11" s="11">
+        <f>ABS(LN(P12/P11))/ABS(LN(L12/L11))</f>
+      </c>
+      <c r="S11" s="11">
+        <f>(LN(P12/P11))/(LN(L12/L11))</f>
       </c>
       <c r="T11" s="7"/>
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
     </row>
-    <row r="12" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
       <c r="A12" s="1"/>
       <c r="B12" s="8" t="s">
         <v>36</v>
@@ -2454,51 +2292,44 @@
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="28" t="s">
+      <c r="G12" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="H12" s="25" t="s">
+      <c r="H12" s="21" t="s">
         <v>33</v>
       </c>
       <c r="I12" s="22">
-        <v>2.614583333333333</v>
+        <v>3.6145833333333335</v>
       </c>
       <c r="J12" s="23">
         <v>1200</v>
       </c>
       <c r="K12" s="23">
-        <f t="shared" si="0"/>
-        <v>72000</v>
+        <f>J12*60</f>
       </c>
       <c r="L12" s="23">
-        <f t="shared" si="1"/>
-        <v>20</v>
+        <f>J12/60</f>
       </c>
       <c r="M12" s="22">
-        <v>2.0694444444444446</v>
+        <v>3.0694444444444446</v>
       </c>
       <c r="N12" s="11">
         <v>0.45</v>
       </c>
       <c r="O12" s="23">
-        <f t="shared" si="6"/>
-        <v>18</v>
+        <f>N12*40</f>
       </c>
       <c r="P12" s="23">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="Q12" s="24">
-        <f t="shared" si="3"/>
-        <v>1.1555555555555561</v>
-      </c>
-      <c r="R12" s="24">
-        <f t="shared" si="4"/>
-        <v>3.6648942359366705</v>
-      </c>
-      <c r="S12" s="24">
-        <f t="shared" si="5"/>
-        <v>3.6648942359366705</v>
+        <f>O12/3</f>
+      </c>
+      <c r="Q12" s="11">
+        <f>ABS(P13-P12)/ABS(L13-L12)</f>
+      </c>
+      <c r="R12" s="11">
+        <f>ABS(LN(P13/P12))/ABS(LN(L13/L12))</f>
+      </c>
+      <c r="S12" s="11">
+        <f>(LN(P13/P12))/(LN(L13/L12))</f>
       </c>
       <c r="T12" s="23">
         <v>0</v>
@@ -2506,74 +2337,67 @@
       <c r="U12" s="1"/>
       <c r="V12" s="1"/>
     </row>
-    <row r="13" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
       <c r="A13" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="11">
-        <v>1.0576000000000001</v>
+        <v>1.0576</v>
       </c>
       <c r="C13" s="11">
-        <v>1.0471999999999999</v>
+        <v>1.0472</v>
       </c>
       <c r="D13" s="11">
-        <v>1.0572999999999999</v>
+        <v>1.0573</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H13" s="25" t="s">
+      <c r="H13" s="21" t="s">
         <v>33</v>
       </c>
       <c r="I13" s="22">
-        <v>2.645833333333333</v>
+        <v>3.6458333333333335</v>
       </c>
       <c r="J13" s="23">
         <v>1245</v>
       </c>
       <c r="K13" s="23">
-        <f t="shared" si="0"/>
-        <v>74700</v>
+        <f>J13*60</f>
       </c>
       <c r="L13" s="11">
-        <f t="shared" si="1"/>
-        <v>20.75</v>
+        <f>J13/60</f>
       </c>
       <c r="M13" s="22">
-        <v>2.0694444444444446</v>
+        <v>3.0694444444444446</v>
       </c>
       <c r="N13" s="11">
-        <v>0.51500000000000001</v>
+        <v>0.515</v>
       </c>
       <c r="O13" s="11">
-        <f t="shared" si="6"/>
-        <v>20.6</v>
+        <f>N13*40</f>
       </c>
       <c r="P13" s="11">
-        <f t="shared" si="2"/>
-        <v>6.8666666666666671</v>
-      </c>
-      <c r="Q13" s="24">
-        <f t="shared" si="3"/>
-        <v>0.33333333333333304</v>
-      </c>
-      <c r="R13" s="24">
-        <f t="shared" si="4"/>
-        <v>1.0071116579248927</v>
-      </c>
-      <c r="S13" s="24">
-        <f t="shared" si="5"/>
-        <v>1.0071116579248927</v>
+        <f>O13/3</f>
+      </c>
+      <c r="Q13" s="11">
+        <f>ABS(P14-P13)/ABS(L14-L13)</f>
+      </c>
+      <c r="R13" s="11">
+        <f>ABS(LN(P14/P13))/ABS(LN(L14/L13))</f>
+      </c>
+      <c r="S13" s="11">
+        <f>(LN(P14/P13))/(LN(L14/L13))</f>
       </c>
       <c r="T13" s="11">
-        <v>-16.100000000000001</v>
+        <v>-16.1</v>
       </c>
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
     </row>
-    <row r="14" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
       <c r="A14" s="12" t="s">
         <v>8</v>
       </c>
@@ -2585,48 +2409,41 @@
       <c r="G14" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H14" s="25" t="s">
+      <c r="H14" s="21" t="s">
         <v>33</v>
       </c>
       <c r="I14" s="22">
-        <v>2.6875</v>
+        <v>3.6875</v>
       </c>
       <c r="J14" s="23">
         <v>1305</v>
       </c>
       <c r="K14" s="23">
-        <f t="shared" si="0"/>
-        <v>78300</v>
+        <f>J14*60</f>
       </c>
       <c r="L14" s="11">
-        <f t="shared" si="1"/>
-        <v>21.75</v>
+        <f>J14/60</f>
       </c>
       <c r="M14" s="22">
-        <v>2.0694444444444446</v>
+        <v>3.0694444444444446</v>
       </c>
       <c r="N14" s="11">
         <v>0.54</v>
       </c>
       <c r="O14" s="11">
-        <f t="shared" si="6"/>
-        <v>21.6</v>
+        <f>N14*40</f>
       </c>
       <c r="P14" s="11">
-        <f t="shared" si="2"/>
-        <v>7.2</v>
-      </c>
-      <c r="Q14" s="24">
-        <f t="shared" si="3"/>
-        <v>2.1333333333333337</v>
-      </c>
-      <c r="R14" s="24">
-        <f t="shared" si="4"/>
-        <v>5.7731520165793855</v>
-      </c>
-      <c r="S14" s="24">
-        <f t="shared" si="5"/>
-        <v>5.7731520165793855</v>
+        <f>O14/3</f>
+      </c>
+      <c r="Q14" s="11">
+        <f>ABS(P15-P14)/ABS(L15-L14)</f>
+      </c>
+      <c r="R14" s="11">
+        <f>ABS(LN(P15/P14))/ABS(LN(L15/L14))</f>
+      </c>
+      <c r="S14" s="11">
+        <f>(LN(P15/P14))/(LN(L15/L14))</f>
       </c>
       <c r="T14" s="11">
         <v>-20.3</v>
@@ -2634,7 +2451,7 @@
       <c r="U14" s="1"/>
       <c r="V14" s="1"/>
     </row>
-    <row r="15" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
       <c r="A15" s="1"/>
       <c r="B15" s="8" t="s">
         <v>42</v>
@@ -2650,48 +2467,41 @@
       <c r="G15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H15" s="25" t="s">
+      <c r="H15" s="21" t="s">
         <v>33</v>
       </c>
       <c r="I15" s="22">
-        <v>2.729166666666667</v>
+        <v>3.7291666666666665</v>
       </c>
       <c r="J15" s="23">
         <v>1365</v>
       </c>
       <c r="K15" s="23">
-        <f t="shared" si="0"/>
-        <v>81900</v>
+        <f>J15*60</f>
       </c>
       <c r="L15" s="11">
-        <f t="shared" si="1"/>
-        <v>22.75</v>
+        <f>J15/60</f>
       </c>
       <c r="M15" s="22">
-        <v>2.0694444444444446</v>
+        <v>3.0694444444444446</v>
       </c>
       <c r="N15" s="11">
         <v>0.7</v>
       </c>
       <c r="O15" s="23">
-        <f t="shared" si="6"/>
-        <v>28</v>
+        <f>N15*40</f>
       </c>
       <c r="P15" s="11">
-        <f t="shared" si="2"/>
-        <v>9.3333333333333339</v>
-      </c>
-      <c r="Q15" s="24">
-        <f t="shared" si="3"/>
-        <v>0.25507246376811626</v>
-      </c>
-      <c r="R15" s="24">
-        <f t="shared" si="4"/>
-        <v>0.64770834284972345</v>
-      </c>
-      <c r="S15" s="24">
-        <f t="shared" si="5"/>
-        <v>0.64770834284972345</v>
+        <f>O15/3</f>
+      </c>
+      <c r="Q15" s="11">
+        <f>ABS(P16-P15)/ABS(L16-L15)</f>
+      </c>
+      <c r="R15" s="11">
+        <f>ABS(LN(P16/P15))/ABS(LN(L16/L15))</f>
+      </c>
+      <c r="S15" s="11">
+        <f>(LN(P16/P15))/(LN(L16/L15))</f>
       </c>
       <c r="T15" s="23">
         <v>-43</v>
@@ -2699,15 +2509,15 @@
       <c r="U15" s="1"/>
       <c r="V15" s="1"/>
     </row>
-    <row r="16" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
       <c r="A16" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="11">
-        <v>1.0536000000000001</v>
+        <v>1.0536</v>
       </c>
       <c r="C16" s="11">
-        <v>1.0530999999999999</v>
+        <v>1.0531</v>
       </c>
       <c r="D16" s="11">
         <v>1.0528</v>
@@ -2717,48 +2527,41 @@
       <c r="G16" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H16" s="25" t="s">
+      <c r="H16" s="21" t="s">
         <v>33</v>
       </c>
       <c r="I16" s="22">
-        <v>2.770833333333333</v>
+        <v>3.7708333333333335</v>
       </c>
       <c r="J16" s="23">
         <v>1710</v>
       </c>
       <c r="K16" s="23">
-        <f t="shared" si="0"/>
-        <v>102600</v>
+        <f>J16*60</f>
       </c>
       <c r="L16" s="11">
-        <f t="shared" si="1"/>
-        <v>28.5</v>
+        <f>J16/60</f>
       </c>
       <c r="M16" s="22">
-        <v>2.0694444444444446</v>
+        <v>3.0694444444444446</v>
       </c>
       <c r="N16" s="11">
         <v>0.81</v>
       </c>
       <c r="O16" s="11">
-        <f t="shared" si="6"/>
-        <v>32.400000000000006</v>
+        <f>N16*40</f>
       </c>
       <c r="P16" s="11">
-        <f t="shared" si="2"/>
-        <v>10.800000000000002</v>
-      </c>
-      <c r="Q16" s="24">
-        <f t="shared" si="3"/>
-        <v>1.5733333333333324</v>
-      </c>
-      <c r="R16" s="24">
-        <f t="shared" si="4"/>
-        <v>3.9435362401171079</v>
-      </c>
-      <c r="S16" s="24">
-        <f t="shared" si="5"/>
-        <v>3.9435362401171079</v>
+        <f>O16/3</f>
+      </c>
+      <c r="Q16" s="11">
+        <f>ABS(P17-P16)/ABS(L17-L16)</f>
+      </c>
+      <c r="R16" s="11">
+        <f>ABS(LN(P17/P16))/ABS(LN(L17/L16))</f>
+      </c>
+      <c r="S16" s="11">
+        <f>(LN(P17/P16))/(LN(L17/L16))</f>
       </c>
       <c r="T16" s="11">
         <v>-60.3</v>
@@ -2766,7 +2569,7 @@
       <c r="U16" s="1"/>
       <c r="V16" s="1"/>
     </row>
-    <row r="17" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
       <c r="A17" s="12" t="s">
         <v>8</v>
       </c>
@@ -2778,48 +2581,41 @@
       <c r="G17" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H17" s="25" t="s">
+      <c r="H17" s="21" t="s">
         <v>33</v>
       </c>
       <c r="I17" s="22">
-        <v>2.8125</v>
+        <v>3.8125</v>
       </c>
       <c r="J17" s="23">
         <v>1770</v>
       </c>
       <c r="K17" s="23">
-        <f t="shared" si="0"/>
-        <v>106200</v>
+        <f>J17*60</f>
       </c>
       <c r="L17" s="11">
-        <f t="shared" si="1"/>
-        <v>29.5</v>
+        <f>J17/60</f>
       </c>
       <c r="M17" s="22">
-        <v>2.0694444444444446</v>
+        <v>3.0694444444444446</v>
       </c>
       <c r="N17" s="11">
-        <v>0.92800000000000005</v>
+        <v>0.928</v>
       </c>
       <c r="O17" s="11">
-        <f t="shared" si="6"/>
-        <v>37.120000000000005</v>
+        <f>N17*40</f>
       </c>
       <c r="P17" s="11">
-        <f t="shared" si="2"/>
-        <v>12.373333333333335</v>
-      </c>
-      <c r="Q17" s="24">
-        <f t="shared" si="3"/>
-        <v>1.4280272108843539</v>
-      </c>
-      <c r="R17" s="24">
-        <f t="shared" si="4"/>
-        <v>2.5372188316163391</v>
-      </c>
-      <c r="S17" s="24">
-        <f t="shared" si="5"/>
-        <v>2.5372188316163391</v>
+        <f>O17/3</f>
+      </c>
+      <c r="Q17" s="11">
+        <f>ABS(P18-P17)/ABS(L18-L17)</f>
+      </c>
+      <c r="R17" s="11">
+        <f>ABS(LN(P18/P17))/ABS(LN(L18/L17))</f>
+      </c>
+      <c r="S17" s="11">
+        <f>(LN(P18/P17))/(LN(L18/L17))</f>
       </c>
       <c r="T17" s="11">
         <v>-87.9</v>
@@ -2827,7 +2623,7 @@
       <c r="U17" s="1"/>
       <c r="V17" s="1"/>
     </row>
-    <row r="18" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
       <c r="A18" s="1"/>
       <c r="B18" s="8" t="s">
         <v>48</v>
@@ -2847,32 +2643,28 @@
         <v>52</v>
       </c>
       <c r="I18" s="22">
-        <v>2.322916666666667</v>
+        <v>3.3229166666666665</v>
       </c>
       <c r="J18" s="23">
         <v>2505</v>
       </c>
       <c r="K18" s="23">
-        <f t="shared" si="0"/>
-        <v>150300</v>
+        <f>J18*60</f>
       </c>
       <c r="L18" s="11">
-        <f t="shared" si="1"/>
-        <v>41.75</v>
-      </c>
-      <c r="M18" s="29" t="s">
+        <f>J18/60</f>
+      </c>
+      <c r="M18" s="22" t="s">
         <v>53</v>
       </c>
       <c r="N18" s="11">
-        <v>0.56000000000000005</v>
+        <v>0.56</v>
       </c>
       <c r="O18" s="11">
         <f>N18*160</f>
-        <v>89.600000000000009</v>
       </c>
       <c r="P18" s="11">
-        <f t="shared" si="2"/>
-        <v>29.866666666666671</v>
+        <f>O18/3</f>
       </c>
       <c r="Q18" s="7"/>
       <c r="R18" s="7"/>
@@ -2883,18 +2675,18 @@
       <c r="U18" s="1"/>
       <c r="V18" s="1"/>
     </row>
-    <row r="19" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
       <c r="A19" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B19" s="11">
-        <v>1.0475000000000001</v>
+        <v>1.0475</v>
       </c>
       <c r="C19" s="11">
-        <v>1.0612999999999999</v>
+        <v>1.0613</v>
       </c>
       <c r="D19" s="11">
-        <v>1.0577000000000001</v>
+        <v>1.0577</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -2915,7 +2707,7 @@
       <c r="U19" s="1"/>
       <c r="V19" s="1"/>
     </row>
-    <row r="20" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
       <c r="A20" s="12" t="s">
         <v>8</v>
       </c>
@@ -2941,7 +2733,7 @@
       <c r="U20" s="1"/>
       <c r="V20" s="1"/>
     </row>
-    <row r="21" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
       <c r="A21" s="1"/>
       <c r="B21" s="8" t="s">
         <v>54</v>
@@ -2957,7 +2749,7 @@
       <c r="G21" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H21" s="30">
+      <c r="H21" s="26">
         <v>45121</v>
       </c>
       <c r="I21" s="5"/>
@@ -2965,9 +2757,8 @@
       <c r="K21" s="6"/>
       <c r="L21" s="11">
         <f>J18/60</f>
-        <v>41.75</v>
-      </c>
-      <c r="M21" s="29" t="s">
+      </c>
+      <c r="M21" s="22" t="s">
         <v>58</v>
       </c>
       <c r="N21" s="11">
@@ -2975,11 +2766,9 @@
       </c>
       <c r="O21" s="11">
         <f>N21*120</f>
-        <v>105.6</v>
       </c>
       <c r="P21" s="11">
         <f>O21/3</f>
-        <v>35.199999999999996</v>
       </c>
       <c r="Q21" s="7"/>
       <c r="R21" s="7"/>
@@ -2988,12 +2777,12 @@
       <c r="U21" s="1"/>
       <c r="V21" s="1"/>
     </row>
-    <row r="22" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
       <c r="A22" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B22" s="11">
-        <v>1.0591999999999999</v>
+        <v>1.0592</v>
       </c>
       <c r="C22" s="11">
         <v>1.0447</v>
@@ -3003,39 +2792,35 @@
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="31" t="s">
+      <c r="G22" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="H22" s="32" t="s">
+      <c r="H22" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="I22" s="33">
-        <v>2.520833333333333</v>
-      </c>
-      <c r="J22" s="34">
+      <c r="I22" s="29">
+        <v>3.5208333333333335</v>
+      </c>
+      <c r="J22" s="30">
         <v>1065</v>
       </c>
       <c r="K22" s="23">
         <f>J22*60</f>
-        <v>63900</v>
       </c>
       <c r="L22" s="11">
         <f>J22/60</f>
-        <v>17.75</v>
-      </c>
-      <c r="M22" s="35">
-        <v>2.0555555555555554</v>
-      </c>
-      <c r="N22" s="36">
-        <v>0.83699999999999997</v>
-      </c>
-      <c r="O22" s="36">
+      </c>
+      <c r="M22" s="31">
+        <v>3.0555555555555554</v>
+      </c>
+      <c r="N22" s="32">
+        <v>0.837</v>
+      </c>
+      <c r="O22" s="32">
         <f>N22*20</f>
-        <v>16.739999999999998</v>
-      </c>
-      <c r="P22" s="36">
+      </c>
+      <c r="P22" s="32">
         <f>O22/3</f>
-        <v>5.5799999999999992</v>
       </c>
       <c r="Q22" s="7"/>
       <c r="R22" s="7"/>
@@ -3044,7 +2829,7 @@
       <c r="U22" s="1"/>
       <c r="V22" s="1"/>
     </row>
-    <row r="23" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
       <c r="A23" s="12" t="s">
         <v>8</v>
       </c>
@@ -3070,7 +2855,7 @@
       <c r="U23" s="1"/>
       <c r="V23" s="1"/>
     </row>
-    <row r="24" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
       <c r="A24" s="1"/>
       <c r="B24" s="8" t="s">
         <v>60</v>
@@ -3100,12 +2885,12 @@
       <c r="U24" s="1"/>
       <c r="V24" s="1"/>
     </row>
-    <row r="25" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
       <c r="A25" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B25" s="11">
-        <v>1.0680000000000001</v>
+        <v>1.068</v>
       </c>
       <c r="C25" s="11">
         <v>1.0627</v>
@@ -3132,7 +2917,7 @@
       <c r="U25" s="1"/>
       <c r="V25" s="1"/>
     </row>
-    <row r="26" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
       <c r="A26" s="12" t="s">
         <v>8</v>
       </c>
@@ -3158,7 +2943,7 @@
       <c r="U26" s="1"/>
       <c r="V26" s="1"/>
     </row>
-    <row r="27" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
       <c r="A27" s="1"/>
       <c r="B27" s="8" t="s">
         <v>63</v>
@@ -3188,7 +2973,7 @@
       <c r="U27" s="1"/>
       <c r="V27" s="1"/>
     </row>
-    <row r="28" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
       <c r="A28" s="10" t="s">
         <v>7</v>
       </c>
@@ -3196,7 +2981,7 @@
         <v>1.0608</v>
       </c>
       <c r="C28" s="11">
-        <v>1.0634999999999999</v>
+        <v>1.0635</v>
       </c>
       <c r="D28" s="11">
         <v>1.048</v>
@@ -3220,7 +3005,7 @@
       <c r="U28" s="1"/>
       <c r="V28" s="1"/>
     </row>
-    <row r="29" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
       <c r="A29" s="12" t="s">
         <v>8</v>
       </c>
@@ -3246,7 +3031,7 @@
       <c r="U29" s="1"/>
       <c r="V29" s="1"/>
     </row>
-    <row r="30" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
       <c r="A30" s="1"/>
       <c r="B30" s="8" t="s">
         <v>66</v>
@@ -3265,7 +3050,7 @@
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
       <c r="L30" s="7"/>
-      <c r="M30" s="29" t="s">
+      <c r="M30" s="22" t="s">
         <v>69</v>
       </c>
       <c r="N30" s="7"/>
@@ -3278,18 +3063,18 @@
       <c r="U30" s="1"/>
       <c r="V30" s="1"/>
     </row>
-    <row r="31" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
       <c r="A31" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B31" s="11">
-        <v>1.0711999999999999</v>
+        <v>1.0712</v>
       </c>
       <c r="C31" s="11">
         <v>1.0642</v>
       </c>
       <c r="D31" s="11">
-        <v>1.0578000000000001</v>
+        <v>1.0578</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -3299,7 +3084,7 @@
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
       <c r="L31" s="7"/>
-      <c r="M31" s="29" t="s">
+      <c r="M31" s="22" t="s">
         <v>70</v>
       </c>
       <c r="N31" s="7"/>
@@ -3312,7 +3097,7 @@
       <c r="U31" s="1"/>
       <c r="V31" s="1"/>
     </row>
-    <row r="32" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
       <c r="A32" s="12" t="s">
         <v>8</v>
       </c>
@@ -3324,29 +3109,29 @@
       <c r="G32" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H32" s="25" t="s">
+      <c r="H32" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="I32" s="37">
-        <v>2.666666666666667</v>
-      </c>
-      <c r="J32" s="37"/>
-      <c r="K32" s="37"/>
-      <c r="L32" s="37"/>
-      <c r="M32" s="37"/>
-      <c r="N32" s="37"/>
-      <c r="O32" s="37"/>
-      <c r="P32" s="37"/>
-      <c r="Q32" s="37"/>
-      <c r="R32" s="37"/>
-      <c r="S32" s="37"/>
+      <c r="I32" s="33">
+        <v>3.6666666666666665</v>
+      </c>
+      <c r="J32" s="33"/>
+      <c r="K32" s="33"/>
+      <c r="L32" s="33"/>
+      <c r="M32" s="33"/>
+      <c r="N32" s="33"/>
+      <c r="O32" s="33"/>
+      <c r="P32" s="33"/>
+      <c r="Q32" s="33"/>
+      <c r="R32" s="33"/>
+      <c r="S32" s="33"/>
       <c r="T32" s="11">
         <v>-23.7</v>
       </c>
       <c r="U32" s="1"/>
       <c r="V32" s="1"/>
     </row>
-    <row r="33" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25">
       <c r="A33" s="1"/>
       <c r="B33" s="8" t="s">
         <v>72</v>
@@ -3362,11 +3147,11 @@
       <c r="G33" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H33" s="25" t="s">
+      <c r="H33" s="21" t="s">
         <v>33</v>
       </c>
       <c r="I33" s="22">
-        <v>2.833333333333333</v>
+        <v>3.8333333333333335</v>
       </c>
       <c r="J33" s="22"/>
       <c r="K33" s="22"/>
@@ -3384,15 +3169,15 @@
       <c r="U33" s="1"/>
       <c r="V33" s="1"/>
     </row>
-    <row r="34" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25">
       <c r="A34" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B34" s="11">
-        <v>1.0619000000000001</v>
+        <v>1.0619</v>
       </c>
       <c r="C34" s="11">
-        <v>1.0630999999999999</v>
+        <v>1.0631</v>
       </c>
       <c r="D34" s="11">
         <v>1.0628</v>
@@ -3416,7 +3201,7 @@
       <c r="U34" s="1"/>
       <c r="V34" s="1"/>
     </row>
-    <row r="35" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25">
       <c r="A35" s="12" t="s">
         <v>8</v>
       </c>
@@ -3442,7 +3227,7 @@
       <c r="U35" s="1"/>
       <c r="V35" s="1"/>
     </row>
-    <row r="36" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25">
       <c r="A36" s="1"/>
       <c r="B36" s="8" t="s">
         <v>75</v>
@@ -3472,7 +3257,7 @@
       <c r="U36" s="1"/>
       <c r="V36" s="1"/>
     </row>
-    <row r="37" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25">
       <c r="A37" s="10" t="s">
         <v>7</v>
       </c>
@@ -3480,7 +3265,7 @@
         <v>1.0568</v>
       </c>
       <c r="C37" s="11">
-        <v>1.0559000000000001</v>
+        <v>1.0559</v>
       </c>
       <c r="D37" s="11">
         <v>1.0606</v>
@@ -3504,7 +3289,7 @@
       <c r="U37" s="1"/>
       <c r="V37" s="1"/>
     </row>
-    <row r="38" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25">
       <c r="A38" s="12" t="s">
         <v>8</v>
       </c>
@@ -3530,7 +3315,7 @@
       <c r="U38" s="1"/>
       <c r="V38" s="1"/>
     </row>
-    <row r="39" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25">
       <c r="A39" s="1"/>
       <c r="B39" s="8" t="s">
         <v>78</v>
@@ -3560,7 +3345,7 @@
       <c r="U39" s="1"/>
       <c r="V39" s="1"/>
     </row>
-    <row r="40" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="17.25">
       <c r="A40" s="10" t="s">
         <v>7</v>
       </c>
@@ -3592,7 +3377,7 @@
       <c r="U40" s="1"/>
       <c r="V40" s="1"/>
     </row>
-    <row r="41" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="17.25">
       <c r="A41" s="12" t="s">
         <v>8</v>
       </c>
@@ -3618,7 +3403,7 @@
       <c r="U41" s="1"/>
       <c r="V41" s="1"/>
     </row>
-    <row r="42" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="17.25">
       <c r="A42" s="1"/>
       <c r="B42" s="8" t="s">
         <v>81</v>
@@ -3648,7 +3433,7 @@
       <c r="U42" s="1"/>
       <c r="V42" s="1"/>
     </row>
-    <row r="43" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="17.25">
       <c r="A43" s="10" t="s">
         <v>7</v>
       </c>
@@ -3674,7 +3459,7 @@
       <c r="U43" s="1"/>
       <c r="V43" s="1"/>
     </row>
-    <row r="44" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="17.25">
       <c r="A44" s="12" t="s">
         <v>8</v>
       </c>
@@ -3700,7 +3485,7 @@
       <c r="U44" s="1"/>
       <c r="V44" s="1"/>
     </row>
-    <row r="45" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="17.25">
       <c r="A45" s="1"/>
       <c r="B45" s="8" t="s">
         <v>84</v>
@@ -3732,9 +3517,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Calibri"&amp;10&amp;K000000 Public&amp;1#_x000D_</oddHeader>
-    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public</oddFooter>
-  </headerFooter>
 </worksheet>
 </file>
</xml_diff>